<commit_message>
Creating Notifications Workflow for SE and BRE
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\700024\Documents\UiPath\Projects\UiPath\SubstituteItems_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424DD1E5-C8F6-4CB7-96F4-337EB58C2FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D078E4-DED6-497D-A26A-ADC38AD52E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="6600" windowWidth="17385" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29055" yWindow="4335" windowWidth="18315" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -186,13 +183,49 @@
     <t>Input - Substitute Items.xlsx</t>
   </si>
   <si>
-    <t>Substitute Items file name</t>
-  </si>
-  <si>
     <t>Substitute Items Sheet name</t>
   </si>
   <si>
     <t>File_SubstituteItemsName</t>
+  </si>
+  <si>
+    <t>Sheet_BuyersName</t>
+  </si>
+  <si>
+    <t>Buyers List</t>
+  </si>
+  <si>
+    <t>Buyers list sheet name</t>
+  </si>
+  <si>
+    <t>Transaction File (Input File)</t>
+  </si>
+  <si>
+    <t>Substitute Items file name (Input file)</t>
+  </si>
+  <si>
+    <t>SubstituteItems.Performer</t>
+  </si>
+  <si>
+    <t>File_NotificationsByBuyersName</t>
+  </si>
+  <si>
+    <t>Notifications By Buyers (Input File)</t>
+  </si>
+  <si>
+    <t>Sheet_NotificationsByBuyersName</t>
+  </si>
+  <si>
+    <t>Buyers</t>
+  </si>
+  <si>
+    <t>Input_NotificationsByBuyers.xlsx</t>
+  </si>
+  <si>
+    <t>Input file - Notifications by Buyers</t>
+  </si>
+  <si>
+    <t>Sheet name - Buyers</t>
   </si>
 </sst>
 </file>
@@ -224,12 +257,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -244,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -254,6 +293,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -618,24 +658,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -644,43 +684,85 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
         <v>50</v>
       </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
         <v>55</v>
       </c>
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" t="s">
-        <v>53</v>
+      <c r="C11" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1663,6 +1745,8 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1728,18 +1812,18 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1763,7 +1847,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1785,7 +1869,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1796,7 +1880,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1807,53 +1891,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2838,7 +2922,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2857,7 +2941,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2887,46 +2971,46 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Creating send notifications file (Buyers and Emails)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\700024\Documents\UiPath\Projects\UiPath\SubstituteItems_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D078E4-DED6-497D-A26A-ADC38AD52E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9351FCC7-C8AF-4E7F-ABAF-47A3D1C554D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29055" yWindow="4335" windowWidth="18315" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28200" yWindow="4950" windowWidth="18315" windowHeight="13050" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -207,25 +207,46 @@
     <t>SubstituteItems.Performer</t>
   </si>
   <si>
-    <t>File_NotificationsByBuyersName</t>
-  </si>
-  <si>
-    <t>Notifications By Buyers (Input File)</t>
-  </si>
-  <si>
-    <t>Sheet_NotificationsByBuyersName</t>
-  </si>
-  <si>
     <t>Buyers</t>
   </si>
   <si>
-    <t>Input_NotificationsByBuyers.xlsx</t>
-  </si>
-  <si>
     <t>Input file - Notifications by Buyers</t>
   </si>
   <si>
-    <t>Sheet name - Buyers</t>
+    <t>Input_SendNotifications (Input File)</t>
+  </si>
+  <si>
+    <t>File_SendNotificationsName</t>
+  </si>
+  <si>
+    <t>Sheet_EmailsName</t>
+  </si>
+  <si>
+    <t>Emails</t>
+  </si>
+  <si>
+    <t>Sheet name for Send Notifications</t>
+  </si>
+  <si>
+    <t>Sheet name for Send Notifications by buyers</t>
+  </si>
+  <si>
+    <t>Input_SendNotifications.xlsx</t>
+  </si>
+  <si>
+    <t>Send SMTP Mail Message</t>
+  </si>
+  <si>
+    <t>EmailSMTPServerPortName</t>
+  </si>
+  <si>
+    <t>10.101.1.126</t>
+  </si>
+  <si>
+    <t>EmailSMTPServerHostName</t>
+  </si>
+  <si>
+    <t>EmailSMTPAccountName</t>
   </si>
 </sst>
 </file>
@@ -283,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -294,6 +315,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -736,49 +760,83 @@
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2921,8 +2979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>